<commit_message>
It is not working right, but applied Column Span successfully.
</commit_message>
<xml_diff>
--- a/TestDrivenDev/TDD_PivotStructure/PivoteerWPF/ProjectSamples/Stocks.xlsx
+++ b/TestDrivenDev/TDD_PivotStructure/PivoteerWPF/ProjectSamples/Stocks.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="89">
   <si>
     <t>Sector</t>
   </si>
@@ -613,15 +613,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
@@ -632,13 +634,13 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -661,13 +663,13 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -690,13 +692,13 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -719,13 +721,13 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -748,13 +750,13 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -777,13 +779,13 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
         <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -806,13 +808,13 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -835,13 +837,13 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -864,30 +866,262 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>2019</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>22</v>
+      </c>
+      <c r="I9">
+        <v>68.88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>2018</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+      <c r="H10">
+        <v>22</v>
+      </c>
+      <c r="I10">
+        <v>73.34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>2018</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>6</v>
+      </c>
+      <c r="H11">
+        <v>22</v>
+      </c>
+      <c r="I11">
+        <v>22.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>2018</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>6</v>
+      </c>
+      <c r="H12">
+        <v>22</v>
+      </c>
+      <c r="I12">
+        <v>13.98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9">
-        <v>2019</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9">
-        <v>8</v>
-      </c>
-      <c r="H9">
-        <v>22</v>
-      </c>
-      <c r="I9">
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>2018</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>6</v>
+      </c>
+      <c r="H13">
+        <v>22</v>
+      </c>
+      <c r="I13">
+        <v>68.88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>2018</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>8</v>
+      </c>
+      <c r="H14">
+        <v>22</v>
+      </c>
+      <c r="I14">
+        <v>73.34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>2018</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>8</v>
+      </c>
+      <c r="H15">
+        <v>22</v>
+      </c>
+      <c r="I15">
+        <v>22.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>2018</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>8</v>
+      </c>
+      <c r="H16">
+        <v>22</v>
+      </c>
+      <c r="I16">
+        <v>13.98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>2018</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <v>8</v>
+      </c>
+      <c r="H17">
+        <v>22</v>
+      </c>
+      <c r="I17">
         <v>68.88</v>
       </c>
     </row>
@@ -900,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I161"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="I161" sqref="I161"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H158" sqref="H158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Add 2 X 3 Testing Class
</commit_message>
<xml_diff>
--- a/TestDrivenDev/TDD_PivotStructure/PivoteerWPF/ProjectSamples/Stocks.xlsx
+++ b/TestDrivenDev/TDD_PivotStructure/PivoteerWPF/ProjectSamples/Stocks.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="89">
   <si>
     <t>Sector</t>
   </si>
@@ -613,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -624,15 +624,14 @@
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="7" max="7" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -643,25 +642,22 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="E1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -671,26 +667,23 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
+      <c r="D2">
+        <v>2019</v>
       </c>
       <c r="E2">
-        <v>2019</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G2">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="H2">
-        <v>22</v>
-      </c>
-      <c r="I2">
         <v>73.34</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -700,26 +693,23 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
+      <c r="D3">
+        <v>2019</v>
       </c>
       <c r="E3">
-        <v>2019</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G3">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="H3">
-        <v>22</v>
-      </c>
-      <c r="I3">
         <v>22.6</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -729,26 +719,23 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
+      <c r="D4">
+        <v>2019</v>
       </c>
       <c r="E4">
-        <v>2019</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G4">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="H4">
-        <v>22</v>
-      </c>
-      <c r="I4">
         <v>13.98</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -758,26 +745,23 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
-        <v>8</v>
+      <c r="D5">
+        <v>2019</v>
       </c>
       <c r="E5">
-        <v>2019</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G5">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="H5">
-        <v>22</v>
-      </c>
-      <c r="I5">
         <v>68.88</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -787,26 +771,23 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
-        <v>8</v>
+      <c r="D6">
+        <v>2019</v>
       </c>
       <c r="E6">
-        <v>2019</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G6">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="H6">
-        <v>22</v>
-      </c>
-      <c r="I6">
         <v>73.34</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -816,26 +797,23 @@
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
-        <v>8</v>
+      <c r="D7">
+        <v>2019</v>
       </c>
       <c r="E7">
-        <v>2019</v>
+        <v>3</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G7">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="H7">
-        <v>22</v>
-      </c>
-      <c r="I7">
         <v>22.6</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -845,26 +823,23 @@
       <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" t="s">
-        <v>8</v>
+      <c r="D8">
+        <v>2019</v>
       </c>
       <c r="E8">
-        <v>2019</v>
+        <v>3</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G8">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="H8">
-        <v>22</v>
-      </c>
-      <c r="I8">
         <v>13.98</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -874,26 +849,23 @@
       <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="D9" t="s">
-        <v>8</v>
+      <c r="D9">
+        <v>2019</v>
       </c>
       <c r="E9">
-        <v>2019</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G9">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="H9">
-        <v>22</v>
-      </c>
-      <c r="I9">
         <v>68.88</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -903,26 +875,23 @@
       <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
-        <v>8</v>
+      <c r="D10">
+        <v>2018</v>
       </c>
       <c r="E10">
-        <v>2018</v>
+        <v>2</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G10">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="H10">
-        <v>22</v>
-      </c>
-      <c r="I10">
         <v>73.34</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -932,26 +901,23 @@
       <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="D11" t="s">
-        <v>8</v>
+      <c r="D11">
+        <v>2018</v>
       </c>
       <c r="E11">
-        <v>2018</v>
+        <v>2</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G11">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="H11">
-        <v>22</v>
-      </c>
-      <c r="I11">
         <v>22.6</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -961,26 +927,23 @@
       <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="D12" t="s">
-        <v>8</v>
+      <c r="D12">
+        <v>2018</v>
       </c>
       <c r="E12">
-        <v>2018</v>
+        <v>2</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G12">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="H12">
-        <v>22</v>
-      </c>
-      <c r="I12">
         <v>13.98</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -990,26 +953,23 @@
       <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="D13" t="s">
-        <v>8</v>
+      <c r="D13">
+        <v>2018</v>
       </c>
       <c r="E13">
-        <v>2018</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G13">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="H13">
-        <v>22</v>
-      </c>
-      <c r="I13">
         <v>68.88</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1019,26 +979,23 @@
       <c r="C14" t="s">
         <v>5</v>
       </c>
-      <c r="D14" t="s">
-        <v>8</v>
+      <c r="D14">
+        <v>2018</v>
       </c>
       <c r="E14">
-        <v>2018</v>
+        <v>3</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G14">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="H14">
-        <v>22</v>
-      </c>
-      <c r="I14">
         <v>73.34</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1048,26 +1005,23 @@
       <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="D15" t="s">
-        <v>8</v>
+      <c r="D15">
+        <v>2018</v>
       </c>
       <c r="E15">
-        <v>2018</v>
+        <v>3</v>
       </c>
       <c r="F15">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G15">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="H15">
-        <v>22</v>
-      </c>
-      <c r="I15">
         <v>22.6</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1077,26 +1031,23 @@
       <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="D16" t="s">
-        <v>8</v>
+      <c r="D16">
+        <v>2018</v>
       </c>
       <c r="E16">
-        <v>2018</v>
+        <v>3</v>
       </c>
       <c r="F16">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G16">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="H16">
-        <v>22</v>
-      </c>
-      <c r="I16">
         <v>13.98</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1106,23 +1057,436 @@
       <c r="C17" t="s">
         <v>14</v>
       </c>
-      <c r="D17" t="s">
-        <v>8</v>
+      <c r="D17">
+        <v>2018</v>
       </c>
       <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>22</v>
+      </c>
+      <c r="H17">
+        <v>68.88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>2019</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>23</v>
+      </c>
+      <c r="H18">
+        <v>74.34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>2019</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>6</v>
+      </c>
+      <c r="G19">
+        <v>23</v>
+      </c>
+      <c r="H19">
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <v>2019</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <v>23</v>
+      </c>
+      <c r="H20">
+        <v>14.98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21">
+        <v>2019</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>6</v>
+      </c>
+      <c r="G21">
+        <v>23</v>
+      </c>
+      <c r="H21">
+        <v>69.88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>2019</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>8</v>
+      </c>
+      <c r="G22">
+        <v>23</v>
+      </c>
+      <c r="H22">
+        <v>78.34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23">
+        <v>2019</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>8</v>
+      </c>
+      <c r="G23">
+        <v>23</v>
+      </c>
+      <c r="H23">
+        <v>21.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24">
+        <v>2019</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>8</v>
+      </c>
+      <c r="G24">
+        <v>23</v>
+      </c>
+      <c r="H24">
+        <v>13.98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25">
+        <v>2019</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>8</v>
+      </c>
+      <c r="G25">
+        <v>23</v>
+      </c>
+      <c r="H25">
+        <v>68.88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26">
         <v>2018</v>
       </c>
-      <c r="F17">
-        <v>3</v>
-      </c>
-      <c r="G17">
-        <v>8</v>
-      </c>
-      <c r="H17">
-        <v>22</v>
-      </c>
-      <c r="I17">
-        <v>68.88</v>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>6</v>
+      </c>
+      <c r="G26">
+        <v>23</v>
+      </c>
+      <c r="H26">
+        <v>73.34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27">
+        <v>2018</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>6</v>
+      </c>
+      <c r="G27">
+        <v>23</v>
+      </c>
+      <c r="H27">
+        <v>22.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28">
+        <v>2018</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>6</v>
+      </c>
+      <c r="G28">
+        <v>23</v>
+      </c>
+      <c r="H28">
+        <v>13.98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29">
+        <v>2018</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>6</v>
+      </c>
+      <c r="G29">
+        <v>23</v>
+      </c>
+      <c r="H29">
+        <v>64.88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>2018</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>8</v>
+      </c>
+      <c r="G30">
+        <v>23</v>
+      </c>
+      <c r="H30">
+        <v>65.34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31">
+        <v>2018</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <v>8</v>
+      </c>
+      <c r="G31">
+        <v>23</v>
+      </c>
+      <c r="H31">
+        <v>22.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32">
+        <v>2018</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <v>8</v>
+      </c>
+      <c r="G32">
+        <v>23</v>
+      </c>
+      <c r="H32">
+        <v>13.98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33">
+        <v>2018</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33">
+        <v>8</v>
+      </c>
+      <c r="G33">
+        <v>23</v>
+      </c>
+      <c r="H33">
+        <v>63.88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>